<commit_message>
start shortest path graph creation
</commit_message>
<xml_diff>
--- a/Capstone_testfile1.xlsx
+++ b/Capstone_testfile1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheil\Documents\University4B\Capstone\FYDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D259A92E-7CCC-47BB-9887-B35942E1D9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED58461-CAB2-446D-8743-BD1141107441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2C28F0EC-D3C5-4116-B35E-2B1143F028FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{2C28F0EC-D3C5-4116-B35E-2B1143F028FC}"/>
   </bookViews>
   <sheets>
     <sheet name="distance" sheetId="2" r:id="rId1"/>
@@ -126,9 +126,6 @@
     <t>gasVDiesel</t>
   </si>
   <si>
-    <t>cost$perKm</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>LookUP_ID</t>
+  </si>
+  <si>
+    <t>costperKm</t>
   </si>
 </sst>
 </file>
@@ -16054,7 +16054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E28A1B1-7502-429F-85F9-CD10DDDC1BB5}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -16065,7 +16065,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -16297,7 +16297,7 @@
   <dimension ref="A1:C1408"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31804,7 +31804,7 @@
   <dimension ref="A1:C1408"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47310,8 +47310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2110C9B-6C2B-4BD2-A9A9-3FC4C1DECE20}">
   <dimension ref="A1:D145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A17:B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47332,7 +47332,7 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -49350,13 +49350,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
shortest path try to build graph for emissions
</commit_message>
<xml_diff>
--- a/Capstone_testfile1.xlsx
+++ b/Capstone_testfile1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheil\Documents\University4B\Capstone\FYDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED58461-CAB2-446D-8743-BD1141107441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6762F2E-EE9F-47CD-AC62-A716C8C156DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{2C28F0EC-D3C5-4116-B35E-2B1143F028FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{2C28F0EC-D3C5-4116-B35E-2B1143F028FC}"/>
   </bookViews>
   <sheets>
     <sheet name="distance" sheetId="2" r:id="rId1"/>
@@ -51,15 +51,6 @@
     <t>currlocation</t>
   </si>
   <si>
-    <t>Origin ID</t>
-  </si>
-  <si>
-    <t>Destination ID</t>
-  </si>
-  <si>
-    <t>Length [m]</t>
-  </si>
-  <si>
     <t>capacity</t>
   </si>
   <si>
@@ -76,12 +67,6 @@
   </si>
   <si>
     <t>demand_units</t>
-  </si>
-  <si>
-    <t>Trip Cost [$]</t>
-  </si>
-  <si>
-    <t>Speed Limit [km/hr]</t>
   </si>
   <si>
     <t>typeTruck</t>
@@ -139,6 +124,21 @@
   </si>
   <si>
     <t>costperKm</t>
+  </si>
+  <si>
+    <t>Speed_Limit</t>
+  </si>
+  <si>
+    <t>Origin_ID</t>
+  </si>
+  <si>
+    <t>Destination_ID</t>
+  </si>
+  <si>
+    <t>Length_m</t>
+  </si>
+  <si>
+    <t>Trip_Cost_dollar</t>
   </si>
 </sst>
 </file>
@@ -547,25 +547,25 @@
   <dimension ref="A1:C1408"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -16065,19 +16065,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -16088,10 +16088,10 @@
         <v>100</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -16102,10 +16102,10 @@
         <v>50</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -16116,10 +16116,10 @@
         <v>50</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -16175,10 +16175,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -16296,8 +16296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662D3964-B315-46AB-B568-DEF1F2961ED0}">
   <dimension ref="A1:C1408"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16306,15 +16306,15 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -31804,7 +31804,7 @@
   <dimension ref="A1:C1408"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31813,15 +31813,15 @@
     <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -47310,7 +47310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2110C9B-6C2B-4BD2-A9A9-3FC4C1DECE20}">
   <dimension ref="A1:D145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -47323,24 +47323,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -47351,10 +47351,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -47365,10 +47365,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -47379,10 +47379,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>30</v>
@@ -47393,10 +47393,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -47407,10 +47407,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>30</v>
@@ -47421,10 +47421,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>30</v>
@@ -47435,10 +47435,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>30</v>
@@ -47449,10 +47449,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>30</v>
@@ -47460,10 +47460,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>30</v>
@@ -47474,10 +47474,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>30</v>
@@ -47488,10 +47488,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C13">
         <v>30</v>
@@ -47502,10 +47502,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>30</v>
@@ -47516,10 +47516,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>30</v>
@@ -47530,10 +47530,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
       </c>
       <c r="C16">
         <v>30</v>
@@ -47544,10 +47544,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <v>30</v>
@@ -47558,10 +47558,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>30</v>
@@ -47572,10 +47572,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>30</v>
@@ -47586,10 +47586,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <v>40</v>
@@ -47600,10 +47600,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <v>40</v>
@@ -47614,10 +47614,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>40</v>
@@ -47628,10 +47628,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C23">
         <v>40</v>
@@ -47642,10 +47642,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
         <v>18</v>
-      </c>
-      <c r="B24" t="s">
-        <v>23</v>
       </c>
       <c r="C24">
         <v>40</v>
@@ -47656,10 +47656,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C25">
         <v>40</v>
@@ -47670,10 +47670,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C26">
         <v>40</v>
@@ -47684,10 +47684,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C27">
         <v>40</v>
@@ -47698,10 +47698,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C28">
         <v>40</v>
@@ -47709,10 +47709,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C29">
         <v>40</v>
@@ -47723,10 +47723,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C30">
         <v>40</v>
@@ -47737,10 +47737,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C31">
         <v>40</v>
@@ -47751,10 +47751,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C32">
         <v>40</v>
@@ -47765,10 +47765,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C33">
         <v>40</v>
@@ -47779,10 +47779,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
         <v>19</v>
-      </c>
-      <c r="B34" t="s">
-        <v>24</v>
       </c>
       <c r="C34">
         <v>40</v>
@@ -47793,10 +47793,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C35">
         <v>40</v>
@@ -47807,10 +47807,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C36">
         <v>40</v>
@@ -47821,10 +47821,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C37">
         <v>40</v>
@@ -47835,10 +47835,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C38">
         <v>50</v>
@@ -47849,10 +47849,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C39">
         <v>50</v>
@@ -47863,10 +47863,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C40">
         <v>50</v>
@@ -47877,10 +47877,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C41">
         <v>50</v>
@@ -47891,10 +47891,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
         <v>18</v>
-      </c>
-      <c r="B42" t="s">
-        <v>23</v>
       </c>
       <c r="C42">
         <v>50</v>
@@ -47905,10 +47905,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C43">
         <v>50</v>
@@ -47919,10 +47919,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C44">
         <v>50</v>
@@ -47933,10 +47933,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C45">
         <v>50</v>
@@ -47947,10 +47947,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C46">
         <v>50</v>
@@ -47958,10 +47958,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C47">
         <v>50</v>
@@ -47972,10 +47972,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C48">
         <v>50</v>
@@ -47986,10 +47986,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C49">
         <v>50</v>
@@ -48000,10 +48000,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C50">
         <v>50</v>
@@ -48014,10 +48014,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C51">
         <v>50</v>
@@ -48028,10 +48028,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
         <v>19</v>
-      </c>
-      <c r="B52" t="s">
-        <v>24</v>
       </c>
       <c r="C52">
         <v>50</v>
@@ -48042,10 +48042,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C53">
         <v>50</v>
@@ -48056,10 +48056,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C54">
         <v>50</v>
@@ -48070,10 +48070,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C55">
         <v>50</v>
@@ -48084,10 +48084,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C56">
         <v>60</v>
@@ -48098,10 +48098,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C57">
         <v>60</v>
@@ -48112,10 +48112,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C58">
         <v>60</v>
@@ -48126,10 +48126,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C59">
         <v>60</v>
@@ -48140,10 +48140,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" t="s">
         <v>18</v>
-      </c>
-      <c r="B60" t="s">
-        <v>23</v>
       </c>
       <c r="C60">
         <v>60</v>
@@ -48154,10 +48154,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C61">
         <v>60</v>
@@ -48168,10 +48168,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B62" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C62">
         <v>60</v>
@@ -48182,10 +48182,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C63">
         <v>60</v>
@@ -48196,10 +48196,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C64">
         <v>60</v>
@@ -48208,10 +48208,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C65">
         <v>60</v>
@@ -48222,10 +48222,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C66">
         <v>60</v>
@@ -48236,10 +48236,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C67">
         <v>60</v>
@@ -48250,10 +48250,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B68" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C68">
         <v>60</v>
@@ -48264,10 +48264,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B69" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C69">
         <v>60</v>
@@ -48278,10 +48278,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70" t="s">
         <v>19</v>
-      </c>
-      <c r="B70" t="s">
-        <v>24</v>
       </c>
       <c r="C70">
         <v>60</v>
@@ -48292,10 +48292,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B71" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C71">
         <v>60</v>
@@ -48306,10 +48306,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C72">
         <v>60</v>
@@ -48320,10 +48320,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C73">
         <v>60</v>
@@ -48334,10 +48334,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C74">
         <v>70</v>
@@ -48348,10 +48348,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C75">
         <v>70</v>
@@ -48362,10 +48362,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C76">
         <v>70</v>
@@ -48376,10 +48376,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C77">
         <v>70</v>
@@ -48390,10 +48390,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78" t="s">
         <v>18</v>
-      </c>
-      <c r="B78" t="s">
-        <v>23</v>
       </c>
       <c r="C78">
         <v>70</v>
@@ -48404,10 +48404,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B79" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C79">
         <v>70</v>
@@ -48418,10 +48418,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B80" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C80">
         <v>70</v>
@@ -48432,10 +48432,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C81">
         <v>70</v>
@@ -48446,10 +48446,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C82">
         <v>70</v>
@@ -48457,10 +48457,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B83" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C83">
         <v>70</v>
@@ -48471,10 +48471,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C84">
         <v>70</v>
@@ -48485,10 +48485,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C85">
         <v>70</v>
@@ -48499,10 +48499,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B86" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C86">
         <v>70</v>
@@ -48513,10 +48513,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B87" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C87">
         <v>70</v>
@@ -48527,10 +48527,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B88" t="s">
         <v>19</v>
-      </c>
-      <c r="B88" t="s">
-        <v>24</v>
       </c>
       <c r="C88">
         <v>70</v>
@@ -48541,10 +48541,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B89" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C89">
         <v>70</v>
@@ -48555,10 +48555,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B90" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C90">
         <v>70</v>
@@ -48569,10 +48569,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C91">
         <v>70</v>
@@ -48583,10 +48583,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B92" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C92">
         <v>80</v>
@@ -48597,10 +48597,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B93" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C93">
         <v>80</v>
@@ -48611,10 +48611,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C94">
         <v>80</v>
@@ -48625,10 +48625,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B95" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C95">
         <v>80</v>
@@ -48639,10 +48639,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B96" t="s">
         <v>18</v>
-      </c>
-      <c r="B96" t="s">
-        <v>23</v>
       </c>
       <c r="C96">
         <v>80</v>
@@ -48653,10 +48653,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B97" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C97">
         <v>80</v>
@@ -48667,10 +48667,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C98">
         <v>80</v>
@@ -48681,10 +48681,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C99">
         <v>80</v>
@@ -48695,10 +48695,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B100" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C100">
         <v>80</v>
@@ -48706,10 +48706,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B101" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C101">
         <v>80</v>
@@ -48720,10 +48720,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B102" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C102">
         <v>80</v>
@@ -48734,10 +48734,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C103">
         <v>80</v>
@@ -48748,10 +48748,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B104" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C104">
         <v>80</v>
@@ -48762,10 +48762,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B105" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C105">
         <v>80</v>
@@ -48776,10 +48776,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B106" t="s">
         <v>19</v>
-      </c>
-      <c r="B106" t="s">
-        <v>24</v>
       </c>
       <c r="C106">
         <v>80</v>
@@ -48790,10 +48790,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B107" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C107">
         <v>80</v>
@@ -48804,10 +48804,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B108" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C108">
         <v>80</v>
@@ -48818,10 +48818,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B109" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C109">
         <v>80</v>
@@ -48832,10 +48832,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B110" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C110">
         <v>90</v>
@@ -48846,10 +48846,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B111" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C111">
         <v>90</v>
@@ -48860,10 +48860,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B112" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C112">
         <v>90</v>
@@ -48874,10 +48874,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B113" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C113">
         <v>90</v>
@@ -48888,10 +48888,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B114" t="s">
         <v>18</v>
-      </c>
-      <c r="B114" t="s">
-        <v>23</v>
       </c>
       <c r="C114">
         <v>90</v>
@@ -48902,10 +48902,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B115" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C115">
         <v>90</v>
@@ -48916,10 +48916,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B116" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C116">
         <v>90</v>
@@ -48930,10 +48930,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B117" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C117">
         <v>90</v>
@@ -48944,10 +48944,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C118">
         <v>90</v>
@@ -48955,10 +48955,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B119" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C119">
         <v>90</v>
@@ -48969,10 +48969,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C120">
         <v>90</v>
@@ -48983,10 +48983,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B121" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C121">
         <v>90</v>
@@ -48997,10 +48997,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B122" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C122">
         <v>90</v>
@@ -49011,10 +49011,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B123" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C123">
         <v>90</v>
@@ -49025,10 +49025,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B124" t="s">
         <v>19</v>
-      </c>
-      <c r="B124" t="s">
-        <v>24</v>
       </c>
       <c r="C124">
         <v>90</v>
@@ -49039,10 +49039,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B125" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C125">
         <v>90</v>
@@ -49053,10 +49053,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B126" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C126">
         <v>90</v>
@@ -49067,10 +49067,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B127" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C127">
         <v>90</v>
@@ -49081,10 +49081,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B128" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C128">
         <v>100</v>
@@ -49095,10 +49095,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B129" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C129">
         <v>100</v>
@@ -49109,10 +49109,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B130" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C130">
         <v>100</v>
@@ -49123,10 +49123,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B131" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C131">
         <v>100</v>
@@ -49137,10 +49137,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B132" t="s">
         <v>18</v>
-      </c>
-      <c r="B132" t="s">
-        <v>23</v>
       </c>
       <c r="C132">
         <v>100</v>
@@ -49151,10 +49151,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B133" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C133">
         <v>100</v>
@@ -49165,10 +49165,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B134" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C134">
         <v>100</v>
@@ -49179,10 +49179,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B135" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C135">
         <v>100</v>
@@ -49193,10 +49193,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B136" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C136">
         <v>100</v>
@@ -49205,10 +49205,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B137" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C137">
         <v>100</v>
@@ -49219,10 +49219,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B138" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C138">
         <v>100</v>
@@ -49233,10 +49233,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B139" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C139">
         <v>100</v>
@@ -49247,10 +49247,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B140" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C140">
         <v>100</v>
@@ -49261,10 +49261,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B141" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C141">
         <v>100</v>
@@ -49275,10 +49275,10 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B142" t="s">
         <v>19</v>
-      </c>
-      <c r="B142" t="s">
-        <v>24</v>
       </c>
       <c r="C142">
         <v>100</v>
@@ -49289,10 +49289,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B143" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C143">
         <v>100</v>
@@ -49303,10 +49303,10 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B144" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C144">
         <v>100</v>
@@ -49317,10 +49317,10 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B145" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C145">
         <v>100</v>
@@ -49350,13 +49350,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
get emissions graph to build
</commit_message>
<xml_diff>
--- a/Capstone_testfile1.xlsx
+++ b/Capstone_testfile1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheil\Documents\University4B\Capstone\FYDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CCCE74-42B8-4983-9039-0B04D526B45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F92807-0933-45D0-B7FB-7B4D9DC4D4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{2C28F0EC-D3C5-4116-B35E-2B1143F028FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{2C28F0EC-D3C5-4116-B35E-2B1143F028FC}"/>
   </bookViews>
   <sheets>
     <sheet name="distance" sheetId="2" r:id="rId1"/>
@@ -31814,8 +31814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C048CC81-CCEF-4B17-B943-888993FA9942}">
   <dimension ref="A1:C1408"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47321,8 +47321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2110C9B-6C2B-4BD2-A9A9-3FC4C1DECE20}">
   <dimension ref="A1:D145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49349,7 +49349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85981391-5AC5-412B-9D88-7A67DDE92F86}">
   <dimension ref="A1:C777"/>
   <sheetViews>
-    <sheetView topLeftCell="A749" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D774" sqref="D774"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add run the model button for better flow
</commit_message>
<xml_diff>
--- a/Capstone_testfile1.xlsx
+++ b/Capstone_testfile1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheil\Documents\University4B\Capstone\FYDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAE8249-2605-4711-9233-591CD13A5402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1B0481-D8FE-462E-B273-59A359D42598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{2C28F0EC-D3C5-4116-B35E-2B1143F028FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2C28F0EC-D3C5-4116-B35E-2B1143F028FC}"/>
   </bookViews>
   <sheets>
     <sheet name="distance" sheetId="2" r:id="rId1"/>
@@ -49,9 +49,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="31">
-  <si>
-    <t>currlocation</t>
-  </si>
   <si>
     <t>capacity</t>
   </si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>lookup_ID</t>
+  </si>
+  <si>
+    <t>clcLocation</t>
   </si>
 </sst>
 </file>
@@ -569,13 +569,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -16075,19 +16075,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -16098,10 +16098,10 @@
         <v>100</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -16112,10 +16112,10 @@
         <v>50</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -16126,10 +16126,10 @@
         <v>50</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -16185,10 +16185,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -16278,10 +16278,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76776BBF-AF5C-485D-93C9-550FE96BCFB8}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16289,11 +16289,13 @@
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
     </row>
@@ -16306,7 +16308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662D3964-B315-46AB-B568-DEF1F2961ED0}">
   <dimension ref="A1:C1408"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -16318,13 +16320,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -31826,13 +31828,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -47334,24 +47336,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -47362,10 +47364,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -47376,10 +47378,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -47390,10 +47392,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>30</v>
@@ -47404,10 +47406,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -47418,10 +47420,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>30</v>
@@ -47432,10 +47434,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>30</v>
@@ -47446,10 +47448,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>30</v>
@@ -47460,10 +47462,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
       </c>
       <c r="C10">
         <v>30</v>
@@ -47471,10 +47473,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>30</v>
@@ -47485,10 +47487,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>30</v>
@@ -47499,10 +47501,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>30</v>
@@ -47513,10 +47515,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>30</v>
@@ -47527,10 +47529,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>30</v>
@@ -47541,10 +47543,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>30</v>
@@ -47555,10 +47557,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>30</v>
@@ -47569,10 +47571,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>30</v>
@@ -47583,10 +47585,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>30</v>
@@ -47597,10 +47599,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>40</v>
@@ -47611,10 +47613,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21">
         <v>40</v>
@@ -47625,10 +47627,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22">
         <v>40</v>
@@ -47639,10 +47641,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23">
         <v>40</v>
@@ -47653,10 +47655,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24">
         <v>40</v>
@@ -47667,10 +47669,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25">
         <v>40</v>
@@ -47681,10 +47683,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26">
         <v>40</v>
@@ -47695,10 +47697,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27">
         <v>40</v>
@@ -47709,10 +47711,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
         <v>17</v>
-      </c>
-      <c r="B28" t="s">
-        <v>18</v>
       </c>
       <c r="C28">
         <v>40</v>
@@ -47720,10 +47722,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29">
         <v>40</v>
@@ -47734,10 +47736,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30">
         <v>40</v>
@@ -47748,10 +47750,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31">
         <v>40</v>
@@ -47762,10 +47764,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32">
         <v>40</v>
@@ -47776,10 +47778,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C33">
         <v>40</v>
@@ -47790,10 +47792,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C34">
         <v>40</v>
@@ -47804,10 +47806,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35">
         <v>40</v>
@@ -47818,10 +47820,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C36">
         <v>40</v>
@@ -47832,10 +47834,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C37">
         <v>40</v>
@@ -47846,10 +47848,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C38">
         <v>50</v>
@@ -47860,10 +47862,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39">
         <v>50</v>
@@ -47874,10 +47876,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C40">
         <v>50</v>
@@ -47888,10 +47890,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C41">
         <v>50</v>
@@ -47902,10 +47904,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C42">
         <v>50</v>
@@ -47916,10 +47918,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C43">
         <v>50</v>
@@ -47930,10 +47932,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C44">
         <v>50</v>
@@ -47944,10 +47946,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C45">
         <v>50</v>
@@ -47958,10 +47960,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" t="s">
         <v>17</v>
-      </c>
-      <c r="B46" t="s">
-        <v>18</v>
       </c>
       <c r="C46">
         <v>50</v>
@@ -47969,10 +47971,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C47">
         <v>50</v>
@@ -47983,10 +47985,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C48">
         <v>50</v>
@@ -47997,10 +47999,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C49">
         <v>50</v>
@@ -48011,10 +48013,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C50">
         <v>50</v>
@@ -48025,10 +48027,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C51">
         <v>50</v>
@@ -48039,10 +48041,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C52">
         <v>50</v>
@@ -48053,10 +48055,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C53">
         <v>50</v>
@@ -48067,10 +48069,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C54">
         <v>50</v>
@@ -48081,10 +48083,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C55">
         <v>50</v>
@@ -48095,10 +48097,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C56">
         <v>60</v>
@@ -48109,10 +48111,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C57">
         <v>60</v>
@@ -48123,10 +48125,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C58">
         <v>60</v>
@@ -48137,10 +48139,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C59">
         <v>60</v>
@@ -48151,10 +48153,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C60">
         <v>60</v>
@@ -48165,10 +48167,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C61">
         <v>60</v>
@@ -48179,10 +48181,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B62" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C62">
         <v>60</v>
@@ -48193,10 +48195,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C63">
         <v>60</v>
@@ -48207,10 +48209,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" t="s">
         <v>17</v>
-      </c>
-      <c r="B64" t="s">
-        <v>18</v>
       </c>
       <c r="C64">
         <v>60</v>
@@ -48219,10 +48221,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C65">
         <v>60</v>
@@ -48233,10 +48235,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C66">
         <v>60</v>
@@ -48247,10 +48249,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C67">
         <v>60</v>
@@ -48261,10 +48263,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C68">
         <v>60</v>
@@ -48275,10 +48277,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C69">
         <v>60</v>
@@ -48289,10 +48291,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B70" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C70">
         <v>60</v>
@@ -48303,10 +48305,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C71">
         <v>60</v>
@@ -48317,10 +48319,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C72">
         <v>60</v>
@@ -48331,10 +48333,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C73">
         <v>60</v>
@@ -48345,10 +48347,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B74" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C74">
         <v>70</v>
@@ -48359,10 +48361,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C75">
         <v>70</v>
@@ -48373,10 +48375,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C76">
         <v>70</v>
@@ -48387,10 +48389,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C77">
         <v>70</v>
@@ -48401,10 +48403,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C78">
         <v>70</v>
@@ -48415,10 +48417,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C79">
         <v>70</v>
@@ -48429,10 +48431,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B80" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C80">
         <v>70</v>
@@ -48443,10 +48445,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B81" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C81">
         <v>70</v>
@@ -48457,10 +48459,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" t="s">
         <v>17</v>
-      </c>
-      <c r="B82" t="s">
-        <v>18</v>
       </c>
       <c r="C82">
         <v>70</v>
@@ -48468,10 +48470,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C83">
         <v>70</v>
@@ -48482,10 +48484,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B84" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C84">
         <v>70</v>
@@ -48496,10 +48498,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C85">
         <v>70</v>
@@ -48510,10 +48512,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C86">
         <v>70</v>
@@ -48524,10 +48526,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B87" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C87">
         <v>70</v>
@@ -48538,10 +48540,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B88" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C88">
         <v>70</v>
@@ -48552,10 +48554,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B89" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C89">
         <v>70</v>
@@ -48566,10 +48568,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B90" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C90">
         <v>70</v>
@@ -48580,10 +48582,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B91" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C91">
         <v>70</v>
@@ -48594,10 +48596,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C92">
         <v>80</v>
@@ -48608,10 +48610,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C93">
         <v>80</v>
@@ -48622,10 +48624,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B94" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C94">
         <v>80</v>
@@ -48636,10 +48638,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B95" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C95">
         <v>80</v>
@@ -48650,10 +48652,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B96" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C96">
         <v>80</v>
@@ -48664,10 +48666,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B97" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C97">
         <v>80</v>
@@ -48678,10 +48680,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B98" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C98">
         <v>80</v>
@@ -48692,10 +48694,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B99" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C99">
         <v>80</v>
@@ -48706,10 +48708,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B100" t="s">
         <v>17</v>
-      </c>
-      <c r="B100" t="s">
-        <v>18</v>
       </c>
       <c r="C100">
         <v>80</v>
@@ -48717,10 +48719,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B101" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C101">
         <v>80</v>
@@ -48731,10 +48733,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B102" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C102">
         <v>80</v>
@@ -48745,10 +48747,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B103" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C103">
         <v>80</v>
@@ -48759,10 +48761,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B104" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C104">
         <v>80</v>
@@ -48773,10 +48775,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B105" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C105">
         <v>80</v>
@@ -48787,10 +48789,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B106" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C106">
         <v>80</v>
@@ -48801,10 +48803,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B107" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C107">
         <v>80</v>
@@ -48815,10 +48817,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B108" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C108">
         <v>80</v>
@@ -48829,10 +48831,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B109" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C109">
         <v>80</v>
@@ -48843,10 +48845,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B110" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C110">
         <v>90</v>
@@ -48857,10 +48859,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B111" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C111">
         <v>90</v>
@@ -48871,10 +48873,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B112" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C112">
         <v>90</v>
@@ -48885,10 +48887,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B113" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C113">
         <v>90</v>
@@ -48899,10 +48901,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B114" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C114">
         <v>90</v>
@@ -48913,10 +48915,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B115" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C115">
         <v>90</v>
@@ -48927,10 +48929,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B116" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C116">
         <v>90</v>
@@ -48941,10 +48943,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B117" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C117">
         <v>90</v>
@@ -48955,10 +48957,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B118" t="s">
         <v>17</v>
-      </c>
-      <c r="B118" t="s">
-        <v>18</v>
       </c>
       <c r="C118">
         <v>90</v>
@@ -48966,10 +48968,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B119" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C119">
         <v>90</v>
@@ -48980,10 +48982,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B120" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C120">
         <v>90</v>
@@ -48994,10 +48996,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C121">
         <v>90</v>
@@ -49008,10 +49010,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B122" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C122">
         <v>90</v>
@@ -49022,10 +49024,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B123" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C123">
         <v>90</v>
@@ -49036,10 +49038,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B124" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C124">
         <v>90</v>
@@ -49050,10 +49052,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B125" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C125">
         <v>90</v>
@@ -49064,10 +49066,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B126" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C126">
         <v>90</v>
@@ -49078,10 +49080,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B127" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C127">
         <v>90</v>
@@ -49092,10 +49094,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B128" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C128">
         <v>100</v>
@@ -49106,10 +49108,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B129" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C129">
         <v>100</v>
@@ -49120,10 +49122,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B130" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C130">
         <v>100</v>
@@ -49134,10 +49136,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B131" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C131">
         <v>100</v>
@@ -49148,10 +49150,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B132" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C132">
         <v>100</v>
@@ -49162,10 +49164,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B133" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C133">
         <v>100</v>
@@ -49176,10 +49178,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B134" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C134">
         <v>100</v>
@@ -49190,10 +49192,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B135" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C135">
         <v>100</v>
@@ -49204,10 +49206,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B136" t="s">
         <v>17</v>
-      </c>
-      <c r="B136" t="s">
-        <v>18</v>
       </c>
       <c r="C136">
         <v>100</v>
@@ -49216,10 +49218,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B137" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C137">
         <v>100</v>
@@ -49230,10 +49232,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B138" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C138">
         <v>100</v>
@@ -49244,10 +49246,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B139" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C139">
         <v>100</v>
@@ -49258,10 +49260,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B140" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C140">
         <v>100</v>
@@ -49272,10 +49274,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B141" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C141">
         <v>100</v>
@@ -49286,10 +49288,10 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B142" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C142">
         <v>100</v>
@@ -49300,10 +49302,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B143" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C143">
         <v>100</v>
@@ -49314,10 +49316,10 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B144" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C144">
         <v>100</v>
@@ -49328,10 +49330,10 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B145" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C145">
         <v>100</v>
@@ -49362,13 +49364,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>